<commit_message>
Refactored code, finished U.I creation
</commit_message>
<xml_diff>
--- a/Data Dictionary/attfire1_assignment2-data_dictionary.xlsx
+++ b/Data Dictionary/attfire1_assignment2-data_dictionary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="117">
   <si>
     <t>Table Name</t>
   </si>
@@ -61,13 +61,7 @@
     <t>EnsembleLevel</t>
   </si>
   <si>
-    <t>EnsembleLevelDesc</t>
-  </si>
-  <si>
     <t>YES</t>
-  </si>
-  <si>
-    <t>An ensemble for beginners</t>
   </si>
   <si>
     <t>People</t>
@@ -1289,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,57 +1379,57 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="5" t="s">
+    <row r="5" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="7">
-        <v>250</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="7">
+        <v>50</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="7">
-        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>20</v>
@@ -1455,19 +1449,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>23</v>
@@ -1475,19 +1469,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="7">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>25</v>
@@ -1495,78 +1489,78 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="7">
-        <v>10</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>27</v>
+        <v>9</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="7">
+      <c r="B14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>8</v>
@@ -1583,10 +1577,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>8</v>
@@ -1601,57 +1595,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="C18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="E19" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>36</v>
@@ -1666,12 +1660,12 @@
         <v>10</v>
       </c>
       <c r="F20" s="7">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>38</v>
@@ -1680,44 +1674,44 @@
         <v>8</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F22" s="7">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>9</v>
@@ -1731,10 +1725,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>8</v>
@@ -1749,105 +1743,105 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="5" t="s">
+    <row r="25" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="C26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
+      <c r="C29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="7">
+        <v>50</v>
+      </c>
+      <c r="F30" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="7">
-        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>48</v>
@@ -1867,7 +1861,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>50</v>
@@ -1879,287 +1873,287 @@
         <v>12</v>
       </c>
       <c r="E32" s="7">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="7">
-        <v>35</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="7">
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F34" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="7">
-        <v>100</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="C38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
+      <c r="C41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B44" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="C44" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="C45" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="7">
+        <v>35</v>
+      </c>
+      <c r="F45" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" s="5" t="s">
+      <c r="B47" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="7">
-        <v>35</v>
-      </c>
-      <c r="F46" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
+      <c r="C47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="C48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="7">
+        <v>50</v>
+      </c>
+      <c r="F48" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F48" s="7">
-        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>66</v>
@@ -2168,86 +2162,86 @@
         <v>8</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="7">
-        <v>50</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>67</v>
+        <v>37</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="7">
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F50" s="7">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B51" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F51" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52" s="7">
+      <c r="B53" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>70</v>
@@ -2256,18 +2250,18 @@
         <v>8</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" s="7">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="E54" s="7">
+        <v>50</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>72</v>
@@ -2279,63 +2273,63 @@
         <v>12</v>
       </c>
       <c r="E55" s="7">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B56" s="5" t="s">
+    <row r="56" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56" s="7">
-        <v>250</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
+      <c r="B57" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="7">
+        <v>35</v>
+      </c>
+      <c r="F58" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58" s="7">
-        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>77</v>
@@ -2347,111 +2341,111 @@
         <v>12</v>
       </c>
       <c r="E59" s="7">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B60" s="5" t="s">
+    <row r="60" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="10"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="7">
-        <v>200</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="10"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
+      <c r="B61" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B63" s="5" t="s">
+      <c r="B64" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F63" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="10"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
+      <c r="C64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="C65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" s="7">
+        <v>35</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F65" s="7">
-        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>85</v>
@@ -2463,7 +2457,7 @@
         <v>12</v>
       </c>
       <c r="E66" s="7">
-        <v>35</v>
+        <v>-1</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>86</v>
@@ -2471,7 +2465,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>87</v>
@@ -2480,154 +2474,154 @@
         <v>8</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E67" s="7">
-        <v>-1</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>88</v>
+        <v>35</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E68" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F68" s="7">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B69" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F69" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F69" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B70" s="5" t="s">
+    </row>
+    <row r="70" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="10"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C70" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E70" s="7">
-        <v>-1</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="10"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
+      <c r="B71" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="10"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F72" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B73" s="5" t="s">
+      <c r="B74" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F73" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="10"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
+      <c r="C74" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="C75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E75" s="7">
+        <v>50</v>
+      </c>
+      <c r="F75" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F75" s="7">
-        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>97</v>
@@ -2636,18 +2630,18 @@
         <v>8</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E76" s="7">
-        <v>50</v>
-      </c>
-      <c r="F76" s="7" t="s">
         <v>98</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="8">
+        <v>41529</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>99</v>
@@ -2661,13 +2655,13 @@
       <c r="E77" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F77" s="8">
-        <v>41529</v>
+      <c r="F77" s="9">
+        <v>0.75</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>101</v>
@@ -2676,140 +2670,140 @@
         <v>8</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E78" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F78" s="9">
-        <v>0.75</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B79" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="10"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C79" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F79" s="9">
-        <v>0.8125</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B80" s="5" t="s">
+      <c r="B81" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F80" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="10"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
+      <c r="C81" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="C82" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="7">
+        <v>50</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="10"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C82" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F82" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B83" s="5" t="s">
+      <c r="B84" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C83" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E83" s="7">
-        <v>50</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="10"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
+      <c r="C84" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="C85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85" s="7">
+        <v>100</v>
+      </c>
+      <c r="F85" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F85" s="7">
-        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>12</v>
@@ -2823,19 +2817,19 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E87" s="7">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="F87" s="7" t="s">
         <v>113</v>
@@ -2843,7 +2837,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>114</v>
@@ -2852,62 +2846,42 @@
         <v>8</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E88" s="7">
-        <v>35</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>115</v>
+        <v>9</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F88" s="7">
+        <v>9012</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B89" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E89" s="7">
+        <v>9</v>
+      </c>
+      <c r="F89" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C89" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F89" s="7">
-        <v>9012</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E90" s="7">
-        <v>9</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="10"/>
-      <c r="B91" s="11"/>
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12"/>
+    </row>
+    <row r="90" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="10"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>